<commit_message>
Add "of the <specific> form type" condition
Didn't realise this required Microsoft InfoPath
</commit_message>
<xml_diff>
--- a/docs/Rules Availability.xlsx
+++ b/docs/Rules Availability.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugh/Documents/GitHub/OutlookRulesReader/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5ED999D-04E8-6F46-B437-E8A94102F78B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28234FF4-C1E7-DF4D-9382-438A1646F267}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15980" xr2:uid="{BDA48E04-717D-AA4C-9675-774E8C952669}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="84">
   <si>
     <t>Conditions</t>
   </si>
@@ -269,6 +269,15 @@
   </si>
   <si>
     <t>Exception</t>
+  </si>
+  <si>
+    <t>of the &lt;specific&gt; form type</t>
+  </si>
+  <si>
+    <t>Note: this requires Microsoft InfoPath to be installed to be creatable.</t>
+  </si>
+  <si>
+    <t>Note: this is removed in Outlook 2003</t>
   </si>
 </sst>
 </file>
@@ -370,7 +379,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="175">
+  <dxfs count="64">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -392,6 +401,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -412,1643 +428,529 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2422,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2345055-2AC4-B64B-9F21-7A0D75DAC00C}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3504,13 +2406,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>7</v>
@@ -3519,25 +2421,27 @@
         <v>6</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I33" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="I33" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="J33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K33" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>7</v>
@@ -3566,10 +2470,47 @@
       <c r="J34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K34" s="7"/>
+      <c r="K34" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J21:J28 B1:C1048576 J32 E32:H32 E33:J1048576 E21:H28 E29:J31 E1:J20">
+  <conditionalFormatting sqref="J21:J28 B1:C1048576 J32:J33 E32:H33 E34:J1048576 E21:H28 E29:J31 E1:J20">
     <cfRule type="cellIs" dxfId="63" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -3586,10 +2527,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4495,232 +3436,232 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B27 A28:B28 A30:B1048576 A1:B26 E30:I1048576 E1:I20 D1 C2:C29 K1:XFD1048576 E22:I28 E21 G21:I21">
-    <cfRule type="cellIs" dxfId="59" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="65" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="66" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:H18">
-    <cfRule type="cellIs" dxfId="56" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:H17">
-    <cfRule type="cellIs" dxfId="54" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="61" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="62" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:H16">
-    <cfRule type="cellIs" dxfId="52" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="59" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="60" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:H19">
-    <cfRule type="cellIs" dxfId="50" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="57" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="58" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27:I27">
-    <cfRule type="cellIs" dxfId="48" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="55" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="56" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:I25">
-    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="53" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="54" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:I28">
-    <cfRule type="cellIs" dxfId="44" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="51" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="52" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="42" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="39" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="cellIs" dxfId="40" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="43" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="41" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="42" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29 E29:I29">
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:I29">
-    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:D1048576 D1:D28">
-    <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="32" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C1048576">
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:J1048576 J1:J28">
-    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27">
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add RWZ Format Business Case
</commit_message>
<xml_diff>
--- a/docs/Rules Availability.xlsx
+++ b/docs/Rules Availability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugh/Documents/GitHub/OutlookRulesReader/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28234FF4-C1E7-DF4D-9382-438A1646F267}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B58C44-93D7-5D4A-85FE-EF773166E48E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15980" xr2:uid="{BDA48E04-717D-AA4C-9675-774E8C952669}"/>
   </bookViews>
@@ -1327,7 +1327,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add Outlook 98-2003 Junk E-Mail condition & action
</commit_message>
<xml_diff>
--- a/docs/Rules Availability.xlsx
+++ b/docs/Rules Availability.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugh/Documents/GitHub/OutlookRulesReader/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B58C44-93D7-5D4A-85FE-EF773166E48E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DDBC9B-931A-234D-87FC-FAFAFDB1133D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15980" xr2:uid="{BDA48E04-717D-AA4C-9675-774E8C952669}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15960" xr2:uid="{BDA48E04-717D-AA4C-9675-774E8C952669}"/>
   </bookViews>
   <sheets>
     <sheet name="Conditions &amp; Exceptions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="87">
   <si>
     <t>Conditions</t>
   </si>
@@ -278,6 +278,16 @@
   </si>
   <si>
     <t>Note: this is removed in Outlook 2003</t>
+  </si>
+  <si>
+    <t>do not search message for commercial or adult content</t>
+  </si>
+  <si>
+    <t>Note: this can't be created through the rule wizard. It requires turning on Junk E-Mail in the Organize view of Outlook.
+This rule element cannot be modified but can be deleted</t>
+  </si>
+  <si>
+    <t>from senders on my &lt;Exception List&gt;</t>
   </si>
 </sst>
 </file>
@@ -379,7 +389,187 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="64">
+  <dxfs count="89">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -428,529 +618,596 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1324,10 +1581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2345055-2AC4-B64B-9F21-7A0D75DAC00C}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2465,7 +2722,7 @@
         <v>64</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>6</v>
@@ -2500,7 +2757,7 @@
         <v>64</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>6</v>
@@ -2509,28 +2766,111 @@
         <v>83</v>
       </c>
     </row>
+    <row r="36" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J21:J28 B1:C1048576 J32:J33 E32:H33 E34:J1048576 E21:H28 E29:J31 E1:J20">
-    <cfRule type="cellIs" dxfId="63" priority="5" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="6" operator="equal">
+  <conditionalFormatting sqref="J21:J28 B1:C35 J32:J33 E32:H33 E21:H28 E29:J31 E1:J20 E37:J1048576 B37:C1048576 E34:J35">
+    <cfRule type="cellIs" dxfId="88" priority="17" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="18" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="cellIs" dxfId="61" priority="3" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="4" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="15" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="16" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D35 D37:D1048576">
+    <cfRule type="cellIs" dxfId="84" priority="13" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="14" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36:C36 E36:G36 J36">
+    <cfRule type="cellIs" dxfId="82" priority="11" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="12" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="cellIs" dxfId="80" priority="9" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="10" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2540,10 +2880,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A743CAA0-6730-8643-BE4C-C9B8B9B3D36F}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="J5" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3434,234 +3774,317 @@
       </c>
       <c r="J29" s="5"/>
     </row>
+    <row r="30" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B27 A28:B28 A30:B1048576 A1:B26 E30:I1048576 E1:I20 D1 C2:C29 K1:XFD1048576 E22:I28 E21 G21:I21">
-    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
+  <conditionalFormatting sqref="B27 A28:B28 A31:B1048576 A1:B26 E31:I1048576 E1:I20 D1 C2:C29 K1:XFD29 E22:I28 E21 G21:I21 K31:XFD1048576">
+    <cfRule type="cellIs" dxfId="78" priority="17" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="65" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="78" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="79" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:H18">
-    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="77" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:H17">
-    <cfRule type="cellIs" dxfId="52" priority="61" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="74" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="75" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:H16">
-    <cfRule type="cellIs" dxfId="50" priority="59" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="73" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:H19">
-    <cfRule type="cellIs" dxfId="48" priority="57" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="71" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27:I27">
-    <cfRule type="cellIs" dxfId="46" priority="55" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="68" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="69" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:I25">
-    <cfRule type="cellIs" dxfId="44" priority="53" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="66" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="67" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:I28">
-    <cfRule type="cellIs" dxfId="42" priority="51" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="65" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="40" priority="39" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="52" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="53" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="58" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="36" priority="43" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="56" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="57" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="34" priority="41" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="54" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29 E29:I29">
-    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="48" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="49" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:I29">
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D1048576 D1:D28">
-    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="46" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="47" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31:D1048576 D1:D28">
+    <cfRule type="cellIs" dxfId="49" priority="44" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C1048576">
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J30:J1048576 J1:J28">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="42" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:C1048576">
+    <cfRule type="cellIs" dxfId="45" priority="40" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="41" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:J1048576 J1:J28">
+    <cfRule type="cellIs" dxfId="43" priority="36" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="37" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="34" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="35" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="32" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="33" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="30" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="31" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
+    <cfRule type="cellIs" dxfId="35" priority="22" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="23" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19">
+    <cfRule type="cellIs" dxfId="33" priority="28" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18">
+    <cfRule type="cellIs" dxfId="31" priority="26" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="cellIs" dxfId="29" priority="24" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="cellIs" dxfId="27" priority="20" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="21" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="19" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30 K30:XFD30">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30 E30:I30">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30:I30">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J19">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J17">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"?"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add alert rule condition
</commit_message>
<xml_diff>
--- a/docs/Rules Availability.xlsx
+++ b/docs/Rules Availability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugh/Documents/GitHub/OutlookRulesReader/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DDBC9B-931A-234D-87FC-FAFAFDB1133D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB4BDF7-2FED-3243-8DD0-F0D26D16B120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15960" xr2:uid="{BDA48E04-717D-AA4C-9675-774E8C952669}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="89">
   <si>
     <t>Conditions</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>from senders on my &lt;Exception List&gt;</t>
+  </si>
+  <si>
+    <t>Note: this can't be created through the rule wizard. It requires the user to setup a Microsoft Office compatible alert source and to create a rule for the alert.</t>
+  </si>
+  <si>
+    <t>which is an &lt;Alert E-mail&gt;</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="89">
+  <dxfs count="101">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1168,6 +1214,86 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1581,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2345055-2AC4-B64B-9F21-7A0D75DAC00C}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2801,8 +2927,91 @@
         <v>85</v>
       </c>
     </row>
+    <row r="37" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J21:J28 B1:C35 J32:J33 E32:H33 E21:H28 E29:J31 E1:J20 E37:J1048576 B37:C1048576 E34:J35">
+  <conditionalFormatting sqref="J21:J28 B1:C35 J32:J33 E32:H33 E21:H28 E29:J31 E1:J20 E38:J1048576 B38:C1048576 E34:J35">
+    <cfRule type="cellIs" dxfId="100" priority="29" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="30" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27">
+    <cfRule type="cellIs" dxfId="98" priority="27" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="28" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D35 D38:D1048576">
+    <cfRule type="cellIs" dxfId="96" priority="25" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="26" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36:C36 E36:G36 J36">
+    <cfRule type="cellIs" dxfId="94" priority="23" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="24" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="cellIs" dxfId="92" priority="21" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="22" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36">
+    <cfRule type="cellIs" dxfId="90" priority="19" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="20" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36">
     <cfRule type="cellIs" dxfId="88" priority="17" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2810,7 +3019,7 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
+  <conditionalFormatting sqref="I36">
     <cfRule type="cellIs" dxfId="86" priority="15" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2818,7 +3027,7 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D35 D37:D1048576">
+  <conditionalFormatting sqref="H36">
     <cfRule type="cellIs" dxfId="84" priority="13" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2826,23 +3035,23 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36:C36 E36:G36 J36">
-    <cfRule type="cellIs" dxfId="82" priority="11" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="12" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="80" priority="9" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="10" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
+  <conditionalFormatting sqref="B37:C37 E37:G37 J37">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K37">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2850,7 +3059,7 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
+  <conditionalFormatting sqref="K37">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2858,7 +3067,7 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
+  <conditionalFormatting sqref="I37">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2866,7 +3075,7 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
+  <conditionalFormatting sqref="H37">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -3808,283 +4017,283 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B27 A28:B28 A31:B1048576 A1:B26 E31:I1048576 E1:I20 D1 C2:C29 K1:XFD29 E22:I28 E21 G21:I21 K31:XFD1048576">
-    <cfRule type="cellIs" dxfId="78" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="17" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="78" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="78" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="79" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:H18">
-    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="76" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="77" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:H17">
-    <cfRule type="cellIs" dxfId="73" priority="74" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="74" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="75" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:H16">
-    <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="72" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="73" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:H19">
-    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="70" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="71" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27:I27">
-    <cfRule type="cellIs" dxfId="67" priority="68" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="68" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="69" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:I25">
-    <cfRule type="cellIs" dxfId="65" priority="66" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="66" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="67" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:I28">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="64" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="65" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="61" priority="52" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="52" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="53" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="cellIs" dxfId="59" priority="58" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="58" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="59" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="57" priority="56" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="56" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="57" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="55" priority="54" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="54" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="55" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29 E29:I29">
-    <cfRule type="cellIs" dxfId="53" priority="48" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="48" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="49" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:I29">
-    <cfRule type="cellIs" dxfId="51" priority="46" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="46" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="47" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D1048576 D1:D28">
-    <cfRule type="cellIs" dxfId="49" priority="44" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="44" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="45" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="cellIs" dxfId="47" priority="42" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="42" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="43" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C1048576">
-    <cfRule type="cellIs" dxfId="45" priority="40" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="40" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="41" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31:J1048576 J1:J28">
-    <cfRule type="cellIs" dxfId="43" priority="36" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="36" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="37" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27">
-    <cfRule type="cellIs" dxfId="41" priority="34" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="34" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="35" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="cellIs" dxfId="39" priority="32" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="32" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="33" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28">
-    <cfRule type="cellIs" dxfId="37" priority="30" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="30" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="31" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="cellIs" dxfId="35" priority="22" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="22" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="23" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19">
-    <cfRule type="cellIs" dxfId="33" priority="28" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="28" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="29" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18">
-    <cfRule type="cellIs" dxfId="31" priority="26" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="cellIs" dxfId="29" priority="24" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="24" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29">
-    <cfRule type="cellIs" dxfId="27" priority="20" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29">
-    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="18" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="19" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="15" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="16" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30 K30:XFD30">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="13" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30 E30:I30">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:I30">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>